<commit_message>
am impartit programul pe fisiere, am adaugat comentarii cu pasul echivalent din PDF, si am adaugat Sistem Tridiagonal si Metoda Jacobi
</commit_message>
<xml_diff>
--- a/CalculNumeric/Prezenta.xlsx
+++ b/CalculNumeric/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2022_2025\CalculNumeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F4026D-C6D3-4515-8250-B1E33D18D08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4091A08-BC57-4E4F-8FE7-13966736EC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +144,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +177,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -312,10 +324,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,8 +368,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -641,7 +656,7 @@
   <dimension ref="B2:R50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -738,7 +753,7 @@
       <c r="C4" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D4" t="b">
+      <c r="D4" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P4" s="9"/>
@@ -806,7 +821,7 @@
       <c r="C8" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D8" t="b">
+      <c r="D8" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P8" s="9"/>
@@ -837,7 +852,7 @@
       <c r="C10" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D10" t="b">
+      <c r="D10" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="9"/>
@@ -854,7 +869,7 @@
       <c r="C11" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D11" t="b">
+      <c r="D11" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="9"/>
@@ -871,7 +886,7 @@
       <c r="C12" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D12" t="b">
+      <c r="D12" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="9"/>
@@ -886,7 +901,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" t="b">
+      <c r="D13" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="9"/>
@@ -901,7 +916,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" t="b">
+      <c r="D14" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="9"/>
@@ -916,7 +931,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" t="b">
+      <c r="D15" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P15" s="9"/>
@@ -976,7 +991,7 @@
         <v>32</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="D19" t="b">
+      <c r="D19" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>

</xml_diff>

<commit_message>
scheletul metodei coardei + suport de lab
</commit_message>
<xml_diff>
--- a/CalculNumeric/Prezenta.xlsx
+++ b/CalculNumeric/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2022_2025\CalculNumeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4091A08-BC57-4E4F-8FE7-13966736EC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62C45F3-AD65-4472-AAD0-C2CAC4F602F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>sapt 1</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Narcis Turani</t>
   </si>
   <si>
-    <t>Rad Paul</t>
-  </si>
-  <si>
     <t>Andrei Bucsa</t>
   </si>
   <si>
@@ -122,6 +119,15 @@
   </si>
   <si>
     <t>Dumitrel Oprea</t>
+  </si>
+  <si>
+    <t>Paul Rad</t>
+  </si>
+  <si>
+    <t>Ionut Porumb</t>
+  </si>
+  <si>
+    <t>Bogdan Rulea</t>
   </si>
 </sst>
 </file>
@@ -328,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -369,12 +375,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -655,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -720,16 +746,16 @@
     </row>
     <row r="3" spans="2:18">
       <c r="B3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -741,283 +767,347 @@
       <c r="O3" s="4"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="10">
-        <f t="shared" ref="Q3:Q12" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>2</v>
       </c>
       <c r="R3" s="11"/>
     </row>
     <row r="4" spans="2:18">
       <c r="B4" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="19" t="b">
-        <v>1</v>
-      </c>
+      <c r="D4" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="10">
-        <f t="shared" si="0"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
         <v>2</v>
       </c>
       <c r="R4" s="12"/>
     </row>
     <row r="5" spans="2:18">
       <c r="B5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="E5" s="19"/>
+      <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <v>1</v>
       </c>
       <c r="R5" s="12"/>
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D6" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="19"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="10">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>2</v>
       </c>
       <c r="R6" s="12"/>
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" t="b">
         <v>1</v>
       </c>
+      <c r="E7" s="19"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <v>1</v>
       </c>
       <c r="R7" s="12"/>
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="14" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="19" t="b">
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <v>3</v>
       </c>
       <c r="R8" s="12"/>
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="10">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>1</v>
       </c>
       <c r="R9" s="12"/>
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="19" t="b">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="E10" s="19"/>
+      <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <v>1</v>
       </c>
       <c r="R10" s="12"/>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="19" t="b">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="10">
-        <f t="shared" si="0"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>2</v>
       </c>
       <c r="R11" s="12"/>
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="19" t="b">
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>3</v>
       </c>
       <c r="R12" s="12"/>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="19" t="b">
-        <v>1</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="19"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="10">
-        <f t="shared" ref="Q13:Q50" si="1">C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>1</v>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>2</v>
       </c>
       <c r="R13" s="12"/>
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D14" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>3</v>
       </c>
       <c r="R14" s="12"/>
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="19" t="b">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="19"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="10">
-        <f t="shared" si="1"/>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
         <v>1</v>
       </c>
       <c r="R15" s="12"/>
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" t="b">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>3</v>
       </c>
       <c r="R16" s="12"/>
     </row>
     <row r="17" spans="2:18">
       <c r="B17" s="14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" t="b">
+      <c r="D17" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>2</v>
       </c>
       <c r="R17" s="12"/>
     </row>
     <row r="18" spans="2:18">
       <c r="B18" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
+      <c r="D18" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="10">
-        <f t="shared" si="1"/>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
         <v>1</v>
       </c>
       <c r="R18" s="12"/>
     </row>
     <row r="19" spans="2:18">
       <c r="B19" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C19" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D19" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>3</v>
       </c>
       <c r="R19" s="12"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="14"/>
+      <c r="B20" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="C20" s="5"/>
+      <c r="D20" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>2</v>
       </c>
       <c r="R20" s="12"/>
     </row>
     <row r="21" spans="2:18">
-      <c r="B21" s="14"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>2</v>
       </c>
       <c r="R21" s="12"/>
     </row>
@@ -1026,7 +1116,7 @@
       <c r="C22" s="5"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q13:Q50" si="0">C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
         <v>0</v>
       </c>
       <c r="R22" s="12"/>
@@ -1036,7 +1126,7 @@
       <c r="C23" s="5"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R23" s="18"/>
@@ -1046,7 +1136,7 @@
       <c r="C24" s="5"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R24" s="12"/>
@@ -1056,7 +1146,7 @@
       <c r="C25" s="5"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R25" s="12"/>
@@ -1066,7 +1156,7 @@
       <c r="C26" s="5"/>
       <c r="P26" s="9"/>
       <c r="Q26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R26" s="12"/>
@@ -1076,7 +1166,7 @@
       <c r="C27" s="5"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R27" s="12"/>
@@ -1086,7 +1176,7 @@
       <c r="C28" s="5"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R28" s="12"/>
@@ -1096,7 +1186,7 @@
       <c r="C29" s="5"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R29" s="12"/>
@@ -1106,7 +1196,7 @@
       <c r="C30" s="5"/>
       <c r="P30" s="9"/>
       <c r="Q30" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R30" s="12"/>
@@ -1116,7 +1206,7 @@
       <c r="C31" s="5"/>
       <c r="P31" s="9"/>
       <c r="Q31" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R31" s="12"/>
@@ -1126,7 +1216,7 @@
       <c r="C32" s="5"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R32" s="12"/>
@@ -1136,7 +1226,7 @@
       <c r="C33" s="5"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R33" s="12"/>
@@ -1146,7 +1236,7 @@
       <c r="C34" s="5"/>
       <c r="P34" s="9"/>
       <c r="Q34" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R34" s="12"/>
@@ -1156,7 +1246,7 @@
       <c r="C35" s="5"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R35" s="12"/>
@@ -1166,7 +1256,7 @@
       <c r="C36" s="5"/>
       <c r="P36" s="9"/>
       <c r="Q36" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R36" s="12"/>
@@ -1176,7 +1266,7 @@
       <c r="C37" s="5"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R37" s="12"/>
@@ -1186,7 +1276,7 @@
       <c r="C38" s="5"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R38" s="12"/>
@@ -1196,7 +1286,7 @@
       <c r="C39" s="5"/>
       <c r="P39" s="9"/>
       <c r="Q39" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R39" s="12"/>
@@ -1206,7 +1296,7 @@
       <c r="C40" s="5"/>
       <c r="P40" s="9"/>
       <c r="Q40" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R40" s="12"/>
@@ -1216,7 +1306,7 @@
       <c r="C41" s="5"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R41" s="12"/>
@@ -1226,7 +1316,7 @@
       <c r="C42" s="5"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1236,7 +1326,7 @@
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1246,7 +1336,7 @@
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1256,7 +1346,7 @@
       <c r="C45" s="5"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1266,7 +1356,7 @@
       <c r="C46" s="5"/>
       <c r="P46" s="9"/>
       <c r="Q46" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1276,7 +1366,7 @@
       <c r="C47" s="5"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1286,7 +1376,7 @@
       <c r="C48" s="5"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1296,7 +1386,7 @@
       <c r="C49" s="5"/>
       <c r="P49" s="9"/>
       <c r="Q49" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R49" s="12"/>
@@ -1318,20 +1408,24 @@
       <c r="O50" s="7"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R50" s="13"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R12">
-    <sortCondition ref="B3:B12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R21">
+    <sortCondition ref="B3:B21"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q50">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Newton interpolare, desenare grafic
</commit_message>
<xml_diff>
--- a/CalculNumeric/Prezenta.xlsx
+++ b/CalculNumeric/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2022_2025\CalculNumeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50F1578-6AAD-46E2-805B-068F20308438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2D6FC5-F1ED-4FEB-AD57-0F2ECBF7F015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K16" sqref="K15:K16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -773,7 +773,9 @@
         <v>1</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="20" t="b">
+        <v>1</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -781,8 +783,8 @@
       <c r="O3" s="4"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="10">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>4</v>
+        <f t="shared" ref="Q3:Q27" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>5</v>
       </c>
       <c r="R3" s="11"/>
     </row>
@@ -799,7 +801,7 @@
       <c r="E4" s="21"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="10">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R4" s="12"/>
@@ -815,7 +817,7 @@
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="10">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R5" s="18"/>
@@ -837,7 +839,7 @@
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="10">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R6" s="12"/>
@@ -854,10 +856,13 @@
       <c r="I7" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="J7" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="10">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R7" s="12"/>
     </row>
@@ -874,7 +879,7 @@
       <c r="E8" s="19"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="10">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R8" s="12"/>
@@ -890,7 +895,7 @@
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="10">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R9" s="12"/>
@@ -909,7 +914,7 @@
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="10">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R10" s="12"/>
@@ -937,10 +942,13 @@
       <c r="I11" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="J11" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="10">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="R11" s="12"/>
     </row>
@@ -955,7 +963,7 @@
       <c r="E12" s="19"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="10">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R12" s="12"/>
@@ -971,7 +979,7 @@
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="10">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R13" s="12"/>
@@ -993,7 +1001,7 @@
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="10">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R14" s="12"/>
@@ -1015,7 +1023,7 @@
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="10">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R15" s="12"/>
@@ -1043,10 +1051,13 @@
       <c r="I16" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="J16" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="10">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="R16" s="12"/>
     </row>
@@ -1070,10 +1081,13 @@
       <c r="I17" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="J17" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="10">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R17" s="12"/>
     </row>
@@ -1097,10 +1111,13 @@
       <c r="I18" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="J18" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="10">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R18" s="12"/>
     </row>
@@ -1114,7 +1131,7 @@
       <c r="E19" s="19"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="10">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R19" s="12"/>
@@ -1141,7 +1158,7 @@
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="10">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R20" s="12"/>
@@ -1160,7 +1177,7 @@
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="10">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R21" s="12"/>
@@ -1179,7 +1196,7 @@
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="10">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R22" s="12"/>
@@ -1195,7 +1212,7 @@
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="10">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R23" s="12"/>
@@ -1214,7 +1231,7 @@
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="10">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R24" s="12"/>
@@ -1242,10 +1259,13 @@
       <c r="I25" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="J25" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="10">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="R25" s="12"/>
     </row>
@@ -1272,7 +1292,7 @@
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="10">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R26" s="12"/>
@@ -1290,7 +1310,7 @@
       <c r="E27" s="19"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="10">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R27" s="12"/>
@@ -1300,7 +1320,7 @@
       <c r="C28" s="5"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="10">
-        <f t="shared" ref="Q26:Q50" si="0">C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" ref="Q28:Q50" si="1">C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
         <v>0</v>
       </c>
       <c r="R28" s="12"/>
@@ -1310,7 +1330,7 @@
       <c r="C29" s="5"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R29" s="12"/>
@@ -1320,7 +1340,7 @@
       <c r="C30" s="5"/>
       <c r="P30" s="9"/>
       <c r="Q30" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R30" s="12"/>
@@ -1330,7 +1350,7 @@
       <c r="C31" s="5"/>
       <c r="P31" s="9"/>
       <c r="Q31" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R31" s="12"/>
@@ -1340,7 +1360,7 @@
       <c r="C32" s="5"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R32" s="12"/>
@@ -1350,7 +1370,7 @@
       <c r="C33" s="5"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R33" s="12"/>
@@ -1360,7 +1380,7 @@
       <c r="C34" s="5"/>
       <c r="P34" s="9"/>
       <c r="Q34" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R34" s="12"/>
@@ -1370,7 +1390,7 @@
       <c r="C35" s="5"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R35" s="12"/>
@@ -1380,7 +1400,7 @@
       <c r="C36" s="5"/>
       <c r="P36" s="9"/>
       <c r="Q36" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R36" s="12"/>
@@ -1390,7 +1410,7 @@
       <c r="C37" s="5"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R37" s="12"/>
@@ -1400,7 +1420,7 @@
       <c r="C38" s="5"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R38" s="12"/>
@@ -1410,7 +1430,7 @@
       <c r="C39" s="5"/>
       <c r="P39" s="9"/>
       <c r="Q39" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R39" s="12"/>
@@ -1420,7 +1440,7 @@
       <c r="C40" s="5"/>
       <c r="P40" s="9"/>
       <c r="Q40" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R40" s="12"/>
@@ -1430,7 +1450,7 @@
       <c r="C41" s="5"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R41" s="12"/>
@@ -1440,7 +1460,7 @@
       <c r="C42" s="5"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1450,7 +1470,7 @@
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1460,7 +1480,7 @@
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1470,7 +1490,7 @@
       <c r="C45" s="5"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1480,7 +1500,7 @@
       <c r="C46" s="5"/>
       <c r="P46" s="9"/>
       <c r="Q46" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1490,7 +1510,7 @@
       <c r="C47" s="5"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1500,7 +1520,7 @@
       <c r="C48" s="5"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1510,7 +1530,7 @@
       <c r="C49" s="5"/>
       <c r="P49" s="9"/>
       <c r="Q49" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R49" s="12"/>
@@ -1532,7 +1552,7 @@
       <c r="O50" s="7"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R50" s="13"/>

</xml_diff>

<commit_message>
suport 11 de laborator
</commit_message>
<xml_diff>
--- a/CalculNumeric/Prezenta.xlsx
+++ b/CalculNumeric/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2022_2025\CalculNumeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64A06B0-5B4E-4371-8EBB-88843296DF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1275C6-E2BA-4886-90DC-DDE37CEE0EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>sapt 1</t>
   </si>
@@ -152,6 +152,24 @@
   </si>
   <si>
     <t>Zsolt Sule</t>
+  </si>
+  <si>
+    <t>George Pecherle</t>
+  </si>
+  <si>
+    <t>Andrei Arva</t>
+  </si>
+  <si>
+    <t>Cristian Popa</t>
+  </si>
+  <si>
+    <t>Ana-Maria Finciuc</t>
+  </si>
+  <si>
+    <t>Victor Putina</t>
+  </si>
+  <si>
+    <t>David Popa</t>
   </si>
 </sst>
 </file>
@@ -358,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -401,6 +419,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -697,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -762,146 +781,152 @@
     </row>
     <row r="3" spans="2:18">
       <c r="B3" s="14" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="20" t="b">
-        <v>1</v>
-      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="20"/>
-      <c r="F3" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="19" t="b">
-        <v>1</v>
-      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="10">
-        <f t="shared" ref="Q3:Q27" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>6</v>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>1</v>
       </c>
       <c r="R3" s="11"/>
     </row>
     <row r="4" spans="2:18">
       <c r="B4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="21"/>
+        <v>45</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="E4" s="19"/>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <v>1</v>
       </c>
       <c r="R4" s="12"/>
     </row>
     <row r="5" spans="2:18">
       <c r="B5" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="E5" s="19"/>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
+      <c r="D5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="22"/>
+      <c r="J5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R5" s="18"/>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <v>7</v>
+      </c>
+      <c r="R5" s="12"/>
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="19" t="b">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="21"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <v>2</v>
       </c>
       <c r="R6" s="12"/>
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5"/>
       <c r="E7" s="19"/>
-      <c r="H7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="b">
+      <c r="G7" t="b">
         <v>1</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R7" s="12"/>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <v>1</v>
+      </c>
+      <c r="R7" s="18"/>
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="19" t="b">
-        <v>1</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="E8" s="19"/>
+      <c r="F8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <v>3</v>
       </c>
       <c r="R8" s="12"/>
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5"/>
       <c r="E9" s="19"/>
+      <c r="H9" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="I9" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19" t="b">
         <v>1</v>
       </c>
       <c r="K9" t="b">
@@ -909,116 +934,83 @@
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <v>4</v>
       </c>
       <c r="R9" s="12"/>
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="14" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
       <c r="E10" s="19"/>
-      <c r="G10" t="b">
+      <c r="L10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <v>1</v>
       </c>
       <c r="R10" s="12"/>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C11" s="5"/>
       <c r="E11" s="19"/>
-      <c r="F11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="K11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="10">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <v>1</v>
       </c>
       <c r="R11" s="12"/>
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" t="b">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="19"/>
-      <c r="K12" t="b">
-        <v>1</v>
-      </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="10">
-        <f t="shared" si="0"/>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
         <v>2</v>
       </c>
       <c r="R12" s="12"/>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="14" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C13" s="5"/>
       <c r="E13" s="19"/>
-      <c r="I13" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" t="b">
+      <c r="L13" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>1</v>
       </c>
       <c r="R13" s="12"/>
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C14" s="5"/>
       <c r="E14" s="19"/>
-      <c r="F14" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="I14" s="19" t="b">
         <v>1</v>
       </c>
@@ -1027,39 +1019,36 @@
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>2</v>
       </c>
       <c r="R14" s="12"/>
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="19"/>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" t="b">
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" t="b">
         <v>1</v>
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <v>3</v>
       </c>
       <c r="R15" s="12"/>
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -1083,115 +1072,89 @@
       <c r="J16" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="K16" t="b">
+      <c r="K16" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="10">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>9</v>
       </c>
       <c r="R16" s="12"/>
     </row>
     <row r="17" spans="2:18">
       <c r="B17" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C17" s="5"/>
       <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="19"/>
-      <c r="G17" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K17" t="b">
+      <c r="K17" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>2</v>
       </c>
       <c r="R17" s="12"/>
     </row>
     <row r="18" spans="2:18">
       <c r="B18" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="19" t="b">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="E18" s="19"/>
-      <c r="F18" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" t="b">
+      <c r="L18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>1</v>
       </c>
       <c r="R18" s="12"/>
     </row>
     <row r="19" spans="2:18">
       <c r="B19" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C19" s="5"/>
       <c r="E19" s="19"/>
+      <c r="I19" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>3</v>
       </c>
       <c r="R19" s="12"/>
     </row>
     <row r="20" spans="2:18">
       <c r="B20" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="19" t="b">
-        <v>1</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="G20" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="H20" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="19" t="b">
         <v>1</v>
       </c>
       <c r="K20" t="b">
@@ -1199,134 +1162,169 @@
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="10">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>4</v>
       </c>
       <c r="R20" s="12"/>
     </row>
     <row r="21" spans="2:18">
       <c r="B21" s="14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C21" s="5"/>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
       <c r="E21" s="19"/>
-      <c r="H21" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="19" t="b">
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>5</v>
       </c>
       <c r="R21" s="12"/>
     </row>
     <row r="22" spans="2:18">
       <c r="B22" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="19" t="b">
+        <v>24</v>
+      </c>
+      <c r="C22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="G22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>9</v>
       </c>
       <c r="R22" s="12"/>
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
       <c r="E23" s="19"/>
       <c r="G23" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="K23" t="b">
+      <c r="H23" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>7</v>
       </c>
       <c r="R23" s="12"/>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C24" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D24" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E24" s="19"/>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" t="b">
+      <c r="F24" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <v>8</v>
       </c>
       <c r="R24" s="12"/>
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="E25" s="19"/>
-      <c r="F25" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" t="b">
-        <v>1</v>
-      </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="10">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>1</v>
       </c>
       <c r="R25" s="12"/>
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D26" s="19" t="b">
         <v>1</v>
       </c>
@@ -1340,124 +1338,230 @@
       <c r="H26" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="I26" s="19" t="b">
+      <c r="K26" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>6</v>
       </c>
       <c r="R26" s="12"/>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="19" t="b">
-        <v>1</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C27" s="5"/>
       <c r="E27" s="19"/>
-      <c r="K27" t="b">
+      <c r="H27" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>4</v>
       </c>
       <c r="R27" s="12"/>
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="14" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="K28" t="b">
+      <c r="D28" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="10">
-        <f t="shared" ref="Q28:Q50" si="1">C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>1</v>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>2</v>
       </c>
       <c r="R28" s="12"/>
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="K29" t="b">
+      <c r="E29" s="19"/>
+      <c r="G29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" t="b">
         <v>1</v>
       </c>
       <c r="P29" s="9"/>
       <c r="Q29" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>3</v>
       </c>
       <c r="R29" s="12"/>
     </row>
     <row r="30" spans="2:18">
-      <c r="B30" s="14"/>
+      <c r="B30" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="C30" s="5"/>
+      <c r="D30" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>4</v>
       </c>
       <c r="R30" s="12"/>
     </row>
     <row r="31" spans="2:18">
-      <c r="B31" s="14"/>
-      <c r="C31" s="5"/>
+      <c r="B31" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>9</v>
       </c>
       <c r="R31" s="12"/>
     </row>
     <row r="32" spans="2:18">
-      <c r="B32" s="14"/>
+      <c r="B32" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="C32" s="5"/>
+      <c r="D32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>7</v>
       </c>
       <c r="R32" s="12"/>
     </row>
     <row r="33" spans="2:18">
-      <c r="B33" s="14"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="19"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>2</v>
       </c>
       <c r="R33" s="12"/>
     </row>
     <row r="34" spans="2:18">
-      <c r="B34" s="14"/>
+      <c r="B34" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="C34" s="5"/>
+      <c r="E34" s="19"/>
+      <c r="L34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>1</v>
       </c>
       <c r="R34" s="12"/>
     </row>
     <row r="35" spans="2:18">
-      <c r="B35" s="14"/>
+      <c r="B35" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="C35" s="5"/>
+      <c r="E35" s="19"/>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+      <c r="L35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>2</v>
       </c>
       <c r="R35" s="12"/>
     </row>
@@ -1466,7 +1570,7 @@
       <c r="C36" s="5"/>
       <c r="P36" s="9"/>
       <c r="Q36" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q28:Q50" si="0">C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
         <v>0</v>
       </c>
       <c r="R36" s="12"/>
@@ -1476,7 +1580,7 @@
       <c r="C37" s="5"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R37" s="12"/>
@@ -1486,7 +1590,7 @@
       <c r="C38" s="5"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R38" s="12"/>
@@ -1496,7 +1600,7 @@
       <c r="C39" s="5"/>
       <c r="P39" s="9"/>
       <c r="Q39" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R39" s="12"/>
@@ -1506,7 +1610,7 @@
       <c r="C40" s="5"/>
       <c r="P40" s="9"/>
       <c r="Q40" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R40" s="12"/>
@@ -1516,7 +1620,7 @@
       <c r="C41" s="5"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R41" s="12"/>
@@ -1526,7 +1630,7 @@
       <c r="C42" s="5"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1536,7 +1640,7 @@
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1546,7 +1650,7 @@
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1556,7 +1660,7 @@
       <c r="C45" s="5"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1566,7 +1670,7 @@
       <c r="C46" s="5"/>
       <c r="P46" s="9"/>
       <c r="Q46" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1576,7 +1680,7 @@
       <c r="C47" s="5"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1586,7 +1690,7 @@
       <c r="C48" s="5"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1596,7 +1700,7 @@
       <c r="C49" s="5"/>
       <c r="P49" s="9"/>
       <c r="Q49" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R49" s="12"/>
@@ -1618,14 +1722,14 @@
       <c r="O50" s="7"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R50" s="13"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R27">
-    <sortCondition ref="B3:B27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R35">
+    <sortCondition ref="B35"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">

</xml_diff>

<commit_message>
suport + preenta + eemplu
</commit_message>
<xml_diff>
--- a/CalculNumeric/Prezenta.xlsx
+++ b/CalculNumeric/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2022_2025\CalculNumeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D334B24-6862-4778-AFD0-E5B029567787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97981757-1B97-453D-AE50-964AA93C40A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -803,12 +803,14 @@
         <v>1</v>
       </c>
       <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="N3" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="O3" s="4"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="10">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>1</v>
+        <f t="shared" ref="Q3:Q38" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>2</v>
       </c>
       <c r="R3" s="11"/>
     </row>
@@ -824,10 +826,13 @@
       <c r="M4" t="b">
         <v>1</v>
       </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="10">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R4" s="12"/>
     </row>
@@ -863,7 +868,7 @@
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="10">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="R5" s="12"/>
@@ -881,7 +886,7 @@
       <c r="E6" s="21"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="10">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R6" s="12"/>
@@ -897,7 +902,7 @@
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="10">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R7" s="18"/>
@@ -919,7 +924,7 @@
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="10">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R8" s="12"/>
@@ -944,7 +949,7 @@
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="10">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R9" s="12"/>
@@ -958,10 +963,13 @@
       <c r="L10" t="b">
         <v>1</v>
       </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="10">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R10" s="12"/>
     </row>
@@ -979,7 +987,7 @@
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="10">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R11" s="12"/>
@@ -995,10 +1003,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="19"/>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="10">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R12" s="12"/>
     </row>
@@ -1016,7 +1027,7 @@
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="10">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R13" s="12"/>
@@ -1038,7 +1049,7 @@
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="10">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R14" s="12"/>
@@ -1063,7 +1074,7 @@
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="10">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R15" s="12"/>
@@ -1103,10 +1114,13 @@
       <c r="M16" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="N16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="10">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="R16" s="12"/>
     </row>
@@ -1121,7 +1135,7 @@
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="10">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R17" s="12"/>
@@ -1143,7 +1157,7 @@
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="10">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R18" s="12"/>
@@ -1167,10 +1181,13 @@
       <c r="M19" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="10">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R19" s="12"/>
     </row>
@@ -1191,7 +1208,7 @@
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="10">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R20" s="12"/>
@@ -1216,7 +1233,7 @@
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="10">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R21" s="12"/>
@@ -1230,10 +1247,13 @@
       <c r="M22" t="b">
         <v>1</v>
       </c>
+      <c r="N22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="10">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R22" s="12"/>
     </row>
@@ -1260,7 +1280,7 @@
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="10">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R23" s="12"/>
@@ -1276,7 +1296,7 @@
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="10">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R24" s="12"/>
@@ -1318,7 +1338,7 @@
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="10">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="R25" s="12"/>
@@ -1352,10 +1372,13 @@
       <c r="M26" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="N26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="10">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="R26" s="12"/>
     </row>
@@ -1391,10 +1414,13 @@
       <c r="M27" t="b">
         <v>1</v>
       </c>
+      <c r="N27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="10">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="R27" s="12"/>
     </row>
@@ -1408,7 +1434,7 @@
       <c r="E28" s="19"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="10">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R28" s="12"/>
@@ -1438,7 +1464,7 @@
       </c>
       <c r="P29" s="9"/>
       <c r="Q29" s="10">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="R29" s="12"/>
@@ -1464,10 +1490,13 @@
       <c r="M30" t="b">
         <v>1</v>
       </c>
+      <c r="N30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="10">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R30" s="12"/>
     </row>
@@ -1485,7 +1514,7 @@
       </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="10">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R31" s="12"/>
@@ -1508,10 +1537,13 @@
       <c r="M32" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="N32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="10">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R32" s="12"/>
     </row>
@@ -1536,10 +1568,13 @@
       <c r="M33" t="b">
         <v>1</v>
       </c>
+      <c r="N33" t="b">
+        <v>1</v>
+      </c>
       <c r="P33" s="9"/>
       <c r="Q33" s="10">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R33" s="12"/>
     </row>
@@ -1578,10 +1613,13 @@
       <c r="M34" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="N34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="10">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="R34" s="12"/>
     </row>
@@ -1615,10 +1653,13 @@
       <c r="M35" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="N35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="10">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="R35" s="12"/>
     </row>
@@ -1633,10 +1674,13 @@
         <v>1</v>
       </c>
       <c r="E36" s="19"/>
+      <c r="N36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="10">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R36" s="12"/>
     </row>
@@ -1649,10 +1693,13 @@
       <c r="L37" t="b">
         <v>1</v>
       </c>
+      <c r="N37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="10">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R37" s="12"/>
     </row>
@@ -1673,7 +1720,7 @@
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="10">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R38" s="12"/>
@@ -1683,7 +1730,7 @@
       <c r="C39" s="5"/>
       <c r="P39" s="9"/>
       <c r="Q39" s="10">
-        <f t="shared" ref="Q36:Q50" si="0">C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" ref="Q39:Q50" si="1">C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
         <v>0</v>
       </c>
       <c r="R39" s="12"/>
@@ -1693,7 +1740,7 @@
       <c r="C40" s="5"/>
       <c r="P40" s="9"/>
       <c r="Q40" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R40" s="12"/>
@@ -1703,7 +1750,7 @@
       <c r="C41" s="5"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R41" s="12"/>
@@ -1713,7 +1760,7 @@
       <c r="C42" s="5"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1723,7 +1770,7 @@
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1733,7 +1780,7 @@
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1743,7 +1790,7 @@
       <c r="C45" s="5"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1753,7 +1800,7 @@
       <c r="C46" s="5"/>
       <c r="P46" s="9"/>
       <c r="Q46" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1763,7 +1810,7 @@
       <c r="C47" s="5"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1773,7 +1820,7 @@
       <c r="C48" s="5"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1783,7 +1830,7 @@
       <c r="C49" s="5"/>
       <c r="P49" s="9"/>
       <c r="Q49" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R49" s="12"/>
@@ -1805,7 +1852,7 @@
       <c r="O50" s="7"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R50" s="13"/>

</xml_diff>

<commit_message>
note si prezente final
</commit_message>
<xml_diff>
--- a/CalculNumeric/Prezenta.xlsx
+++ b/CalculNumeric/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2022_2025\CalculNumeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A2B3B4-13EE-4D74-BF9D-5978CE0D32AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757810E3-0188-4F3C-8E21-8F4F6812F0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>sapt 1</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Luca Cioara</t>
+  </si>
+  <si>
+    <t>Stefan Lucuta</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,6 +437,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -731,7 +735,7 @@
   <dimension ref="B2:R50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -813,12 +817,16 @@
         <v>1</v>
       </c>
       <c r="O3" s="4"/>
-      <c r="P3" s="8"/>
+      <c r="P3" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="Q3" s="10">
-        <f t="shared" ref="Q3:Q39" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>2</v>
-      </c>
-      <c r="R3" s="11"/>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>3</v>
+      </c>
+      <c r="R3" s="11">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="2:18">
       <c r="B4" s="14" t="s">
@@ -837,10 +845,12 @@
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R4" s="12"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <v>3</v>
+      </c>
+      <c r="R4" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="2:18">
       <c r="B5" s="14" t="s">
@@ -877,10 +887,12 @@
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="10">
-        <f t="shared" si="0"/>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
         <v>9</v>
       </c>
-      <c r="R5" s="12"/>
+      <c r="R5" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="14" t="s">
@@ -898,10 +910,12 @@
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R6" s="12"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <v>3</v>
+      </c>
+      <c r="R6" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="14" t="s">
@@ -912,12 +926,19 @@
       <c r="G7" t="b">
         <v>1</v>
       </c>
-      <c r="P7" s="9"/>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q7" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R7" s="18"/>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <v>3</v>
+      </c>
+      <c r="R7" s="18">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="14" t="s">
@@ -936,10 +957,12 @@
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R8" s="12"/>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <v>3</v>
+      </c>
+      <c r="R8" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="14" t="s">
@@ -961,10 +984,12 @@
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="10">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>4</v>
       </c>
-      <c r="R9" s="12"/>
+      <c r="R9" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="14" t="s">
@@ -978,12 +1003,16 @@
       <c r="N10" t="b">
         <v>1</v>
       </c>
-      <c r="P10" s="9"/>
+      <c r="P10" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q10" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R10" s="12"/>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <v>3</v>
+      </c>
+      <c r="R10" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="14" t="s">
@@ -1000,12 +1029,16 @@
       <c r="N11" t="b">
         <v>1</v>
       </c>
-      <c r="P11" s="9"/>
+      <c r="P11" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q11" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R11" s="12"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <v>4</v>
+      </c>
+      <c r="R11" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="14" t="s">
@@ -1021,12 +1054,16 @@
       <c r="N12" t="b">
         <v>1</v>
       </c>
-      <c r="P12" s="9"/>
+      <c r="P12" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q12" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R12" s="12"/>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>4</v>
+      </c>
+      <c r="R12" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="14" t="s">
@@ -1045,10 +1082,12 @@
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R13" s="12"/>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>3</v>
+      </c>
+      <c r="R13" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="14" t="s">
@@ -1067,10 +1106,12 @@
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R14" s="12"/>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>3</v>
+      </c>
+      <c r="R14" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="14" t="s">
@@ -1090,12 +1131,16 @@
       <c r="M15" t="b">
         <v>1</v>
       </c>
-      <c r="P15" s="9"/>
+      <c r="P15" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q15" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R15" s="12"/>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <v>5</v>
+      </c>
+      <c r="R15" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="14" t="s">
@@ -1138,12 +1183,16 @@
       <c r="O16" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="P16" s="9"/>
+      <c r="P16" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q16" s="10">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="R16" s="12"/>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>13</v>
+      </c>
+      <c r="R16" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="2:18">
       <c r="B17" s="14" t="s">
@@ -1154,12 +1203,19 @@
       <c r="M17" t="b">
         <v>1</v>
       </c>
-      <c r="P17" s="9"/>
+      <c r="O17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q17" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R17" s="12"/>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>3</v>
+      </c>
+      <c r="R17" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="2:18">
       <c r="B18" s="14" t="s">
@@ -1178,10 +1234,12 @@
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R18" s="12"/>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>3</v>
+      </c>
+      <c r="R18" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="2:18">
       <c r="B19" s="14" t="s">
@@ -1207,10 +1265,12 @@
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R19" s="12"/>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>3</v>
+      </c>
+      <c r="R19" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="2:18">
       <c r="B20" s="14" t="s">
@@ -1229,10 +1289,12 @@
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R20" s="12"/>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>3</v>
+      </c>
+      <c r="R20" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="2:18">
       <c r="B21" s="14" t="s">
@@ -1254,10 +1316,12 @@
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="10">
-        <f t="shared" si="0"/>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
         <v>4</v>
       </c>
-      <c r="R21" s="12"/>
+      <c r="R21" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="2:18">
       <c r="B22" s="14" t="s">
@@ -1271,16 +1335,20 @@
       <c r="N22" t="b">
         <v>1</v>
       </c>
-      <c r="P22" s="9"/>
+      <c r="P22" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q22" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R22" s="12"/>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>3</v>
+      </c>
+      <c r="R22" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="5"/>
       <c r="E23" s="19"/>
@@ -1290,102 +1358,96 @@
       <c r="O23" t="b">
         <v>1</v>
       </c>
-      <c r="P23" s="9"/>
+      <c r="P23" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q23" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R23" s="12"/>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>3</v>
+      </c>
+      <c r="R23" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="14" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
       <c r="E24" s="19"/>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" t="b">
-        <v>1</v>
-      </c>
-      <c r="L24" t="b">
-        <v>1</v>
-      </c>
-      <c r="P24" s="9"/>
+      <c r="N24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O24" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q24" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="R24" s="12"/>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <v>3</v>
+      </c>
+      <c r="R24" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="14" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C25" s="5"/>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
       <c r="E25" s="19"/>
-      <c r="M25" t="b">
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R25" s="12"/>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>5</v>
+      </c>
+      <c r="R25" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="E26" s="19"/>
-      <c r="F26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="L26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="P26" s="9"/>
+      <c r="M26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O26" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q26" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="R26" s="12"/>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>3</v>
+      </c>
+      <c r="R26" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -1394,6 +1456,9 @@
         <v>1</v>
       </c>
       <c r="E27" s="19"/>
+      <c r="F27" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="G27" s="19" t="b">
         <v>1</v>
       </c>
@@ -1409,34 +1474,33 @@
       <c r="K27" s="19" t="b">
         <v>1</v>
       </c>
+      <c r="L27" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="M27" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="N27" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="O27" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="10">
-        <f t="shared" si="0"/>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
         <v>10</v>
       </c>
-      <c r="R27" s="12"/>
+      <c r="R27" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D28" s="19" t="b">
+      <c r="D28" t="b">
         <v>1</v>
       </c>
       <c r="E28" s="19"/>
-      <c r="F28" s="19" t="b">
+      <c r="G28" s="19" t="b">
         <v>1</v>
       </c>
       <c r="H28" s="19" t="b">
@@ -1451,10 +1515,7 @@
       <c r="K28" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="L28" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M28" t="b">
+      <c r="M28" s="19" t="b">
         <v>1</v>
       </c>
       <c r="N28" s="19" t="b">
@@ -1465,262 +1526,263 @@
       </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="10">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="R28" s="12"/>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>10</v>
+      </c>
+      <c r="R28" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="14" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D29" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="E29" s="19"/>
-      <c r="P29" s="9"/>
+      <c r="F29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
+      <c r="N29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O29" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q29" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R29" s="12"/>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>12</v>
+      </c>
+      <c r="R29" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="2:18">
       <c r="B30" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D30" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="E30" s="19"/>
-      <c r="F30" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K30" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R30" s="12"/>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>1</v>
+      </c>
+      <c r="R30" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="2:18">
       <c r="B31" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C31" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="E31" s="19"/>
+      <c r="F31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="H31" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="I31" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="K31" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="L31" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M31" t="b">
-        <v>1</v>
-      </c>
-      <c r="N31" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="O31" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R31" s="12"/>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>6</v>
+      </c>
+      <c r="R31" s="12">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="2:18">
       <c r="B32" s="14" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="E32" s="19"/>
-      <c r="F32" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="P32" s="9"/>
+      <c r="H32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M32" t="b">
+        <v>1</v>
+      </c>
+      <c r="N32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P32" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q32" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R32" s="12"/>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>8</v>
+      </c>
+      <c r="R32" s="12">
+        <v>9</v>
+      </c>
     </row>
     <row r="33" spans="2:18">
       <c r="B33" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C33" s="5"/>
+      <c r="D33" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="E33" s="19"/>
-      <c r="G33" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K33" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="L33" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M33" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="N33" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="P33" s="9"/>
+      <c r="F33" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q33" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="R33" s="12"/>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>3</v>
+      </c>
+      <c r="R33" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="2:18">
       <c r="B34" s="14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="E34" s="19"/>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-      <c r="K34" t="b">
-        <v>1</v>
-      </c>
-      <c r="L34" t="b">
-        <v>1</v>
-      </c>
-      <c r="M34" t="b">
-        <v>1</v>
-      </c>
-      <c r="N34" t="b">
+      <c r="G34" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L34" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M34" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N34" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R34" s="12"/>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>5</v>
+      </c>
+      <c r="R34" s="12">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="2:18">
       <c r="B35" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C35" s="5"/>
       <c r="D35" s="19" t="b">
         <v>1</v>
       </c>
       <c r="E35" s="19"/>
-      <c r="F35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="L35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="N35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="O35" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="P35" s="9"/>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+      <c r="L35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
+      <c r="N35" t="b">
+        <v>1</v>
+      </c>
+      <c r="P35" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q35" s="10">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="R35" s="12"/>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>7</v>
+      </c>
+      <c r="R35" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="2:18">
       <c r="B36" s="14" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="E36" s="19"/>
-      <c r="F36" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K36" t="b">
-        <v>1</v>
-      </c>
-      <c r="L36" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M36" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="N36" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="O36" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="P36" s="9"/>
+      <c r="N36" t="b">
+        <v>1</v>
+      </c>
+      <c r="O36" t="b">
+        <v>1</v>
+      </c>
+      <c r="P36" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q36" s="10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="R36" s="12"/>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <v>3</v>
+      </c>
+      <c r="R36" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="2:18">
       <c r="B37" s="14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -1729,88 +1791,170 @@
         <v>1</v>
       </c>
       <c r="E37" s="19"/>
+      <c r="F37" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L37" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M37" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="N37" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="P37" s="9"/>
+      <c r="O37" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P37" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q37" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R37" s="12"/>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>13</v>
+      </c>
+      <c r="R37" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="2:18">
       <c r="B38" s="14" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C38" s="5"/>
+      <c r="D38" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="E38" s="19"/>
-      <c r="L38" t="b">
-        <v>1</v>
-      </c>
-      <c r="N38" t="b">
-        <v>1</v>
-      </c>
-      <c r="P38" s="9"/>
+      <c r="F38" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+      <c r="L38" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N38" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O38" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q38" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R38" s="12"/>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <v>11</v>
+      </c>
+      <c r="R38" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="2:18">
       <c r="B39" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C39" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="E39" s="19"/>
-      <c r="K39" t="b">
-        <v>1</v>
-      </c>
-      <c r="L39" t="b">
-        <v>1</v>
-      </c>
-      <c r="M39" t="b">
+      <c r="N39" s="19" t="b">
         <v>1</v>
       </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="10">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R39" s="12"/>
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>3</v>
+      </c>
+      <c r="R39" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="2:18">
       <c r="B40" s="14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="O40" t="b">
-        <v>1</v>
-      </c>
-      <c r="P40" s="9"/>
+      <c r="E40" s="19"/>
+      <c r="L40" t="b">
+        <v>1</v>
+      </c>
+      <c r="N40" t="b">
+        <v>1</v>
+      </c>
+      <c r="P40" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q40" s="10">
-        <f t="shared" ref="Q40:Q50" si="1">C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
-        <v>1</v>
-      </c>
-      <c r="R40" s="12"/>
+        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <v>3</v>
+      </c>
+      <c r="R40" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="2:18">
-      <c r="B41" s="14"/>
+      <c r="B41" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="C41" s="5"/>
+      <c r="E41" s="19"/>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" t="b">
+        <v>1</v>
+      </c>
+      <c r="M41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R41" s="12"/>
+        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <v>3</v>
+      </c>
+      <c r="R41" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="2:18">
       <c r="B42" s="14"/>
       <c r="C42" s="5"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q40:Q50" si="0">C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1820,7 +1964,7 @@
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1830,7 +1974,7 @@
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1840,7 +1984,7 @@
       <c r="C45" s="5"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1850,7 +1994,7 @@
       <c r="C46" s="5"/>
       <c r="P46" s="9"/>
       <c r="Q46" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1860,7 +2004,7 @@
       <c r="C47" s="5"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1870,7 +2014,7 @@
       <c r="C48" s="5"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1880,7 +2024,7 @@
       <c r="C49" s="5"/>
       <c r="P49" s="9"/>
       <c r="Q49" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R49" s="12"/>
@@ -1902,14 +2046,14 @@
       <c r="O50" s="7"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R50" s="13"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R39">
-    <sortCondition ref="B39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R41">
+    <sortCondition ref="B41"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">

</xml_diff>